<commit_message>
add new products in google sheets
</commit_message>
<xml_diff>
--- a/new_sku_data.xlsx
+++ b/new_sku_data.xlsx
@@ -28,13 +28,13 @@
     <t>SAN15</t>
   </si>
   <si>
-    <t>California Gold Nutrition, омега-3, рыбий жир премиального качества, 240 капсул из рыбьего желатина</t>
+    <t>898220013302</t>
   </si>
   <si>
     <t>SAN939653</t>
   </si>
   <si>
-    <t>Now Foods, Цинк 50мг, 250 таблеток</t>
+    <t>733739015228</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
add new data main sheets file
</commit_message>
<xml_diff>
--- a/new_sku_data.xlsx
+++ b/new_sku_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>SKU</t>
   </si>
@@ -35,6 +35,42 @@
   </si>
   <si>
     <t>733739015228</t>
+  </si>
+  <si>
+    <t>101454368_4725004</t>
+  </si>
+  <si>
+    <t>898220010325</t>
+  </si>
+  <si>
+    <t>SAN84010</t>
+  </si>
+  <si>
+    <t>306969054093</t>
+  </si>
+  <si>
+    <t>SAN0939547</t>
+  </si>
+  <si>
+    <t>728177004613</t>
+  </si>
+  <si>
+    <t>100918697_4725004</t>
+  </si>
+  <si>
+    <t>898220010332</t>
+  </si>
+  <si>
+    <t>SAN83999</t>
+  </si>
+  <si>
+    <t>733739003706</t>
+  </si>
+  <si>
+    <t>SAN10</t>
+  </si>
+  <si>
+    <t>733739016539</t>
   </si>
 </sst>
 </file>
@@ -402,7 +438,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -443,7 +479,73 @@
         <v>6</v>
       </c>
       <c r="C3" s="2">
-        <v>4821.97</v>
+        <v>4854.94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2">
+        <v>14130.82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2">
+        <v>6005.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2">
+        <v>9839.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2">
+        <v>6863.54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3162.85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2">
+        <v>14054.09</v>
       </c>
     </row>
   </sheetData>

</xml_diff>